<commit_message>
Update Parameters and slicers.xlsx
</commit_message>
<xml_diff>
--- a/Used Fiat 500 in Italy/Parameters and slicers.xlsx
+++ b/Used Fiat 500 in Italy/Parameters and slicers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renate\Documents\GitHub\Python-in-Power-BI\Used Fiat 500 in Italy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF9C5A2E-2152-4E50-BF9B-12416B116E4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F9C4F-5025-42AC-A49A-E562426801AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{90C72EE0-0099-43EE-AE64-D3C322C5C9A6}"/>
   </bookViews>
@@ -168,8 +168,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD8AE008-97A9-4BA6-8550-36D7E711AFCF}" name="Model" displayName="Model" ref="D1:E5" totalsRowShown="0">
-  <autoFilter ref="D1:E5" xr:uid="{283506A0-3F05-4CBF-82F9-CA9438DA0364}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD8AE008-97A9-4BA6-8550-36D7E711AFCF}" name="Model" displayName="Model" ref="C1:D5" totalsRowShown="0">
+  <autoFilter ref="C1:D5" xr:uid="{283506A0-3F05-4CBF-82F9-CA9438DA0364}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9100DAB1-1A51-411C-830B-F8525D59EF28}" name="Model"/>
     <tableColumn id="2" xr3:uid="{696D36CD-4DF9-4D1A-B1B1-5BFC4034F23C}" name="model_no"/>
@@ -179,8 +179,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{116B99E3-A4A3-4291-9669-874BBE08661D}" name="Transmission" displayName="Transmission" ref="G1:H3" totalsRowShown="0">
-  <autoFilter ref="G1:H3" xr:uid="{0C2C0EC5-3CD4-4D56-8A83-967C2D09DDDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{116B99E3-A4A3-4291-9669-874BBE08661D}" name="Transmission" displayName="Transmission" ref="F1:G3" totalsRowShown="0">
+  <autoFilter ref="F1:G3" xr:uid="{0C2C0EC5-3CD4-4D56-8A83-967C2D09DDDB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{DD62C50C-3271-4A37-AF8E-5FAA88B25760}" name="Transmission"/>
     <tableColumn id="2" xr3:uid="{D80E2D88-32E0-4ACF-9143-9B88B45E3412}" name="Transmission_no"/>
@@ -562,90 +562,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85E2FE1-AD81-4F42-92F2-942316E66421}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
         <v>13</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
       <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>69</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
+      <c r="G3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>99</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>101</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>

</xml_diff>